<commit_message>
1.ConfigComponent加载方式调整 2.机器人Console创建命令: CreateRobot --Num=10
</commit_message>
<xml_diff>
--- a/Excel/StartProcessConfig.xlsx
+++ b/Excel/StartProcessConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15980"/>
+    <workbookView windowWidth="26520" windowHeight="14300"/>
   </bookViews>
   <sheets>
     <sheet name="StartProcessConfig" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
   <si>
     <t>Id</t>
   </si>
@@ -25,13 +25,28 @@
     <t>内网端口</t>
   </si>
   <si>
+    <t>程序名</t>
+  </si>
+  <si>
     <t>MachineId</t>
   </si>
   <si>
     <t>InnerPort</t>
   </si>
   <si>
+    <t>AppName</t>
+  </si>
+  <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Server.App</t>
+  </si>
+  <si>
+    <t>Robot.App</t>
   </si>
 </sst>
 </file>
@@ -39,10 +54,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -67,6 +82,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -78,13 +108,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -92,6 +115,13 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -103,9 +133,77 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -120,90 +218,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,13 +247,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,31 +301,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,133 +427,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,6 +438,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -441,20 +465,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -476,26 +497,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,6 +509,17 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,148 +541,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1034,21 +1049,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="C3:E7"/>
+  <dimension ref="C3:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="21.125" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="2" customWidth="1"/>
     <col min="3" max="5" width="12.625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="2"/>
+    <col min="6" max="6" width="14.4134615384615" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5">
+    <row r="3" spans="3:6">
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1058,30 +1074,39 @@
       <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="3:5">
+    <row r="4" spans="3:6">
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="3:6">
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="3:5">
+    <row r="6" s="1" customFormat="1" spans="3:6">
       <c r="C6" s="5">
         <v>1</v>
       </c>
@@ -1091,8 +1116,11 @@
       <c r="E6" s="5">
         <v>20001</v>
       </c>
+      <c r="F6" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="7" spans="3:5">
+    <row r="7" spans="3:6">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -1101,6 +1129,9 @@
       </c>
       <c r="E7" s="5">
         <v>20002</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>